<commit_message>
Update Swastika Skills Audit.xlsx
</commit_message>
<xml_diff>
--- a/Skill Audit/Swastika Skills Audit.xlsx
+++ b/Skill Audit/Swastika Skills Audit.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4507"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22430"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sakri\Documents\GitHub\Group3\Skill Audit\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F2885CE-1DD5-43F7-98CA-ED935CE0880E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19320" windowHeight="11760" tabRatio="500"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -201,8 +207,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="5">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -780,7 +786,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
@@ -790,19 +796,19 @@
       <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="8.5" customWidth="1"/>
     <col min="2" max="2" width="17.5" customWidth="1"/>
     <col min="3" max="3" width="15.5" customWidth="1"/>
-    <col min="4" max="4" width="32.125" customWidth="1"/>
-    <col min="5" max="5" width="32.375" customWidth="1"/>
-    <col min="6" max="6" width="13.125" customWidth="1"/>
-    <col min="7" max="7" width="27.125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="21.875" customWidth="1"/>
+    <col min="4" max="4" width="32.09765625" customWidth="1"/>
+    <col min="5" max="5" width="32.3984375" customWidth="1"/>
+    <col min="6" max="6" width="13.09765625" customWidth="1"/>
+    <col min="7" max="7" width="27.09765625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="21.8984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" s="12" t="s">
         <v>21</v>
       </c>
@@ -814,7 +820,7 @@
       <c r="G1" s="13"/>
       <c r="H1" s="14"/>
     </row>
-    <row r="2" spans="1:8" ht="15" customHeight="1">
+    <row r="2" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="15"/>
       <c r="B2" s="16"/>
       <c r="C2" s="16"/>
@@ -824,7 +830,7 @@
       <c r="G2" s="16"/>
       <c r="H2" s="17"/>
     </row>
-    <row r="3" spans="1:8" ht="15" customHeight="1">
+    <row r="3" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="2"/>
       <c r="B3" s="3"/>
       <c r="C3" s="3"/>
@@ -836,7 +842,7 @@
       </c>
       <c r="H3" s="20"/>
     </row>
-    <row r="4" spans="1:8" ht="15" customHeight="1">
+    <row r="4" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="2"/>
       <c r="B4" s="18" t="s">
         <v>28</v>
@@ -852,7 +858,7 @@
       <c r="G4" s="21"/>
       <c r="H4" s="22"/>
     </row>
-    <row r="5" spans="1:8" ht="15" customHeight="1">
+    <row r="5" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="2"/>
       <c r="B5" s="3"/>
       <c r="C5" s="3"/>
@@ -862,7 +868,7 @@
       <c r="G5" s="21"/>
       <c r="H5" s="22"/>
     </row>
-    <row r="6" spans="1:8">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" s="5" t="s">
         <v>0</v>
       </c>
@@ -888,7 +894,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="60" customHeight="1">
+    <row r="7" spans="1:8" ht="60" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="6">
         <v>1</v>
       </c>
@@ -914,7 +920,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="31.5">
+    <row r="8" spans="1:8" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A8" s="6">
         <v>2</v>
       </c>
@@ -940,7 +946,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="47.25">
+    <row r="9" spans="1:8" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A9" s="6">
         <v>3</v>
       </c>
@@ -966,7 +972,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="31.5">
+    <row r="10" spans="1:8" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A10" s="6">
         <v>4</v>
       </c>
@@ -992,7 +998,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="31.5">
+    <row r="11" spans="1:8" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A11" s="6">
         <v>5</v>
       </c>
@@ -1018,7 +1024,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="31.5">
+    <row r="12" spans="1:8" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A12" s="6">
         <v>6</v>
       </c>
@@ -1044,7 +1050,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="13" spans="1:8" ht="31.5">
+    <row r="13" spans="1:8" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A13" s="6">
         <v>7</v>
       </c>
@@ -1070,7 +1076,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="14" spans="1:8" ht="31.5">
+    <row r="14" spans="1:8" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A14" s="6">
         <v>8</v>
       </c>
@@ -1096,7 +1102,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="15" spans="1:8" ht="47.25">
+    <row r="15" spans="1:8" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A15" s="6">
         <v>9</v>
       </c>
@@ -1122,7 +1128,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="16" spans="1:8" ht="31.5" customHeight="1">
+    <row r="16" spans="1:8" ht="31.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="6">
         <v>10</v>
       </c>
@@ -1148,7 +1154,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="17" spans="1:8" ht="31.5">
+    <row r="17" spans="1:8" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A17" s="1">
         <v>11</v>
       </c>
@@ -1174,7 +1180,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="18" spans="1:8" ht="31.5">
+    <row r="18" spans="1:8" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A18" s="1">
         <v>12</v>
       </c>
@@ -1200,7 +1206,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="19" spans="1:8" ht="31.5">
+    <row r="19" spans="1:8" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A19" s="1">
         <v>13</v>
       </c>
@@ -1226,7 +1232,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="20" spans="1:8" ht="31.5">
+    <row r="20" spans="1:8" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A20" s="1">
         <v>14</v>
       </c>
@@ -1252,7 +1258,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="21" spans="1:8" ht="31.5">
+    <row r="21" spans="1:8" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A21" s="1">
         <v>15</v>
       </c>
@@ -1278,7 +1284,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="22" spans="1:8">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A22" s="1"/>
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
@@ -1288,7 +1294,7 @@
       <c r="G22" s="1"/>
       <c r="H22" s="1"/>
     </row>
-    <row r="23" spans="1:8">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A23" s="1"/>
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
@@ -1298,7 +1304,7 @@
       <c r="G23" s="1"/>
       <c r="H23" s="1"/>
     </row>
-    <row r="24" spans="1:8">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A24" s="1"/>
       <c r="B24" s="1"/>
       <c r="C24" s="1"/>
@@ -1308,7 +1314,7 @@
       <c r="G24" s="1"/>
       <c r="H24" s="1"/>
     </row>
-    <row r="25" spans="1:8">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A25" s="1"/>
       <c r="B25" s="1"/>
       <c r="C25" s="1"/>
@@ -1318,7 +1324,7 @@
       <c r="G25" s="1"/>
       <c r="H25" s="1"/>
     </row>
-    <row r="26" spans="1:8">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A26" s="1"/>
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>

</xml_diff>